<commit_message>
[GPR] Adequação das cores do Quadro de Gerenciamento de Riscos
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Quadro de Gerenciamento de Risco.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Quadro de Gerenciamento de Risco.xlsx
@@ -1,37 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25808"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moises\Dropbox\UFG\5º Período\Projeto Integrador\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Processo Aplicado\EveRemind\2-Gerencia de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29260" windowHeight="15940"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="29265" windowHeight="15945"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="4" r:id="rId1"/>
     <sheet name="Grafico" sheetId="5" r:id="rId2"/>
-    <sheet name="Valores" sheetId="7" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="Acao">Valores!#REF!</definedName>
-    <definedName name="EAR">Valores!#REF!</definedName>
-    <definedName name="Impacto">Valores!$D$3:$D$6</definedName>
+    <definedName name="Acao">#REF!</definedName>
+    <definedName name="EAR">#REF!</definedName>
+    <definedName name="Impacto">#REF!</definedName>
     <definedName name="Importancia">[1]Parametros!$F$2:$F$7</definedName>
     <definedName name="NotaIdeia">[1]Parametros!$E$2:$E$6</definedName>
     <definedName name="Notas">[1]Parametros!$H$2:$H$11</definedName>
-    <definedName name="Prioridade">Valores!#REF!</definedName>
-    <definedName name="Probabilidade">Valores!$C$3:$C$6</definedName>
-    <definedName name="Status">Valores!#REF!</definedName>
-    <definedName name="Urgencia">Valores!#REF!</definedName>
+    <definedName name="Prioridade">#REF!</definedName>
+    <definedName name="Probabilidade">#REF!</definedName>
+    <definedName name="Status">#REF!</definedName>
+    <definedName name="Urgencia">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <webPublishing codePage="1252"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -315,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,6 +535,36 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -787,7 +816,7 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -818,13 +847,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -845,68 +868,239 @@
     <xf numFmtId="0" fontId="20" fillId="37" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="41" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="58">
-    <cellStyle name="Accent1" xfId="1" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent1 - 20%" xfId="2"/>
     <cellStyle name="Accent1 - 20% 2" xfId="45"/>
     <cellStyle name="Accent1 - 40%" xfId="3"/>
     <cellStyle name="Accent1 - 40% 2" xfId="46"/>
     <cellStyle name="Accent1 - 60%" xfId="4"/>
-    <cellStyle name="Accent2" xfId="5" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 - 20%" xfId="6"/>
     <cellStyle name="Accent2 - 20% 2" xfId="47"/>
     <cellStyle name="Accent2 - 40%" xfId="7"/>
     <cellStyle name="Accent2 - 40% 2" xfId="48"/>
     <cellStyle name="Accent2 - 60%" xfId="8"/>
-    <cellStyle name="Accent3" xfId="9" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 - 20%" xfId="10"/>
     <cellStyle name="Accent3 - 20% 2" xfId="49"/>
     <cellStyle name="Accent3 - 40%" xfId="11"/>
     <cellStyle name="Accent3 - 40% 2" xfId="50"/>
     <cellStyle name="Accent3 - 60%" xfId="12"/>
-    <cellStyle name="Accent4" xfId="13" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 - 20%" xfId="14"/>
     <cellStyle name="Accent4 - 20% 2" xfId="51"/>
     <cellStyle name="Accent4 - 40%" xfId="15"/>
     <cellStyle name="Accent4 - 40% 2" xfId="52"/>
     <cellStyle name="Accent4 - 60%" xfId="16"/>
-    <cellStyle name="Accent5" xfId="17" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 - 20%" xfId="18"/>
     <cellStyle name="Accent5 - 20% 2" xfId="53"/>
     <cellStyle name="Accent5 - 40%" xfId="19"/>
     <cellStyle name="Accent5 - 40% 2" xfId="54"/>
     <cellStyle name="Accent5 - 60%" xfId="20"/>
-    <cellStyle name="Accent6" xfId="21" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 - 20%" xfId="22"/>
     <cellStyle name="Accent6 - 20% 2" xfId="55"/>
     <cellStyle name="Accent6 - 40%" xfId="23"/>
     <cellStyle name="Accent6 - 40% 2" xfId="56"/>
     <cellStyle name="Accent6 - 60%" xfId="24"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="31" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula de Verificação" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Célula Vinculada" xfId="37" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Emphasis 1" xfId="28"/>
     <cellStyle name="Emphasis 2" xfId="29"/>
     <cellStyle name="Emphasis 3" xfId="30"/>
-    <cellStyle name="Good" xfId="31" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="32" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="33" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="35" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="36" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="37" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="38" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Ênfase1" xfId="1" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Ênfase2" xfId="5" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Ênfase3" xfId="9" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Ênfase4" xfId="13" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Ênfase5" xfId="17" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Ênfase6" xfId="21" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="36" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorreto" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutra" xfId="38" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="44"/>
-    <cellStyle name="Note" xfId="39" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="40" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="39" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Percent 2" xfId="57"/>
+    <cellStyle name="Saída" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Sheet Title" xfId="41"/>
+    <cellStyle name="Texto de Aviso" xfId="43" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="32" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="33" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="34" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="35" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="100">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1918,603 +2112,603 @@
   <dimension ref="B1:G23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="25.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="55.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="4"/>
       <c r="D1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="B3" s="20">
+    <row r="3" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="17">
         <f t="shared" ref="C3:C17" si="0">$E3+$F3</f>
         <v>5</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="19">
         <v>3</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="19">
         <v>2</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="B4" s="21">
+    <row r="4" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="19">
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="19">
         <v>1</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="19">
         <v>2</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.15">
-      <c r="B5" s="21">
+    <row r="5" spans="2:7" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="B5" s="19">
         <f t="shared" ref="B5:B17" si="1">B4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
         <v>1</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="19">
         <v>2</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.15">
-      <c r="B6" s="21">
+    <row r="6" spans="2:7" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="B6" s="19">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>1</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="19">
         <v>3</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B7" s="21">
+    <row r="7" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B7" s="19">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>3</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="19">
         <v>3</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B8" s="21">
+    <row r="8" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B8" s="19">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="17">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="19">
         <v>1</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="19">
         <v>1</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B9" s="21">
+    <row r="9" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B9" s="19">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
         <v>2</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="19">
         <v>3</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B10" s="21">
+    <row r="10" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B10" s="19">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="19">
         <v>3</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="19">
         <v>1</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B11" s="21">
+    <row r="11" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="B11" s="19">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="19">
         <v>2</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="19">
         <v>3</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
-      <c r="B12" s="21">
+    <row r="12" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="B12" s="19">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="19">
         <v>3</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="19">
         <v>3</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="21">
+    <row r="13" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="19">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="21">
+    <row r="14" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="19">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="21">
+    <row r="15" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="19">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="21">
+    <row r="16" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="19">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
-    <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="21">
+    <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="19">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="79" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="74" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="75" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="76" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="77" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="78" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="74" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="69" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="70" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="71" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="71" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="72" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="72" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="73" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="69" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="64" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="65" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="66" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="66" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="67" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="67" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="68" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="64" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="59" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="60" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="61" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="61" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="62" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="62" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="63" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="63" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="59" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="54" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="55" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="56" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="57" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="58" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="54" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="49" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="50" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="51" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="52" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="52" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="53" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="49" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="44" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="45" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="46" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="47" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="48" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="44" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="39" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="40" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="41" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="42" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="43" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="43" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="39" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="34" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="35" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="36" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="37" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="38" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="38" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="29" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="30" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="31" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="32" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="33" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="24" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="25" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="26" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="27" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="28" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="20" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="21" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="22" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="23" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="14" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="15" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="16" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="17" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="18" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="10" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="11" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="12" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="13" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="7" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="8" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2529,30 +2723,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="1"/>
+    <col min="3" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="28.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="G2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <f>B4+1</f>
         <v>3</v>
@@ -2569,8 +2776,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="G3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <f>B5+1</f>
         <v>2</v>
@@ -2587,8 +2799,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -2604,8 +2825,17 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="G5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2620,25 +2850,52 @@
         <f>D6+1</f>
         <v>3</v>
       </c>
+      <c r="G6" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:E5">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2649,96 +2906,4 @@
     <oddFooter>&amp;L&amp;FPMO Escritório de Projetos&amp;RPágina &amp;P de &amp;Nhttp://escritoriodeprojetos.com.br</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="X9" workbookViewId="0">
-      <selection activeCell="AQ33" sqref="AQ33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.31496062992125984" right="0.35433070866141736" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;LPlano de gerenciamento dos riscos&amp;R&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;FPMO Escritório de Projetos&amp;RPágina &amp;P de &amp;Nhttp://escritoriodeprojetos.com.br</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[GPR] Atualizando o quadro de riscos.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Quadro de Gerenciamento de Risco.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Quadro de Gerenciamento de Risco.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25924"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moises\Dropbox\UFG\5º Período\Projeto Integrador\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Processo Aplicado\EveRemind\2-Gerencia de Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="29265" windowHeight="15945"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29440" windowHeight="19900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="4" r:id="rId1"/>
     <sheet name="Grafico" sheetId="5" r:id="rId2"/>
+    <sheet name="Correções" sheetId="6" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="Acao">#REF!</definedName>
@@ -30,7 +31,7 @@
     <definedName name="Status">#REF!</definedName>
     <definedName name="Urgencia">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <webPublishing codePage="1252"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Severidade</t>
   </si>
@@ -149,6 +150,19 @@
   </si>
   <si>
     <t>Algum membro pode não cumprir o que for alocado para o mesmo realizar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os riscos do projeto serão analisados seguindo critérios referentes ao seu nível de prioridade. 
+Esse critério se baseia na soma dos valores de Impacto e Probabilidade que podem ser de 1 a 3.
+Temos então os níveis de prioridades divididos em 3 níveis respectivamente:
+• Baixa – Valor 1 ou 2
+• Média – Valor 3 ou 4
+• Alta – Valor 5 ou 6
+Temos estratégias corretivas definidas para cada nível de prioridade de risco, sendo elas:
+Prioridade Baixa: Devem ser corrigidos dentro do prazo de 1 Sprint após ser diagnosticado e após a correção deve ser monitorado para evitar que volte a ocorrer.
+Prioridade Média: O responsável pela área de processo deve ter proposto uma opção de correção que deve ser analisada junto ao Gerente de Projeto e se aprovada, deve ser monitorada diariamente para que seja corrigida no prazo de uma semana e atualizado no Quadro de Gerenciamento de Riscos após ser devidamente corrigido.
+Prioridade Alta: O responsável pela área de processo deve ter proposto uma opção de correção que deve ser analisada junto ao Gerente de Projeto e se aprovada, deve ser monitorada diariamente para que seja corrigida o mais rápido possível e atualizado no Quadro de Gerenciamento de Riscos após ser devidamente corrigido.
+</t>
   </si>
 </sst>
 </file>
@@ -158,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -312,6 +326,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="43">
@@ -816,7 +834,7 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -865,9 +883,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -887,220 +902,77 @@
     <xf numFmtId="0" fontId="21" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="58">
+    <cellStyle name="Accent1" xfId="1" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent1 - 20%" xfId="2"/>
     <cellStyle name="Accent1 - 20% 2" xfId="45"/>
     <cellStyle name="Accent1 - 40%" xfId="3"/>
     <cellStyle name="Accent1 - 40% 2" xfId="46"/>
     <cellStyle name="Accent1 - 60%" xfId="4"/>
+    <cellStyle name="Accent2" xfId="5" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 - 20%" xfId="6"/>
     <cellStyle name="Accent2 - 20% 2" xfId="47"/>
     <cellStyle name="Accent2 - 40%" xfId="7"/>
     <cellStyle name="Accent2 - 40% 2" xfId="48"/>
     <cellStyle name="Accent2 - 60%" xfId="8"/>
+    <cellStyle name="Accent3" xfId="9" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 - 20%" xfId="10"/>
     <cellStyle name="Accent3 - 20% 2" xfId="49"/>
     <cellStyle name="Accent3 - 40%" xfId="11"/>
     <cellStyle name="Accent3 - 40% 2" xfId="50"/>
     <cellStyle name="Accent3 - 60%" xfId="12"/>
+    <cellStyle name="Accent4" xfId="13" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 - 20%" xfId="14"/>
     <cellStyle name="Accent4 - 20% 2" xfId="51"/>
     <cellStyle name="Accent4 - 40%" xfId="15"/>
     <cellStyle name="Accent4 - 40% 2" xfId="52"/>
     <cellStyle name="Accent4 - 60%" xfId="16"/>
+    <cellStyle name="Accent5" xfId="17" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 - 20%" xfId="18"/>
     <cellStyle name="Accent5 - 20% 2" xfId="53"/>
     <cellStyle name="Accent5 - 40%" xfId="19"/>
     <cellStyle name="Accent5 - 40% 2" xfId="54"/>
     <cellStyle name="Accent5 - 60%" xfId="20"/>
+    <cellStyle name="Accent6" xfId="21" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 - 20%" xfId="22"/>
     <cellStyle name="Accent6 - 20% 2" xfId="55"/>
     <cellStyle name="Accent6 - 40%" xfId="23"/>
     <cellStyle name="Accent6 - 40% 2" xfId="56"/>
     <cellStyle name="Accent6 - 60%" xfId="24"/>
-    <cellStyle name="Bom" xfId="31" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Célula Vinculada" xfId="37" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Emphasis 1" xfId="28"/>
     <cellStyle name="Emphasis 2" xfId="29"/>
     <cellStyle name="Emphasis 3" xfId="30"/>
-    <cellStyle name="Ênfase1" xfId="1" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="5" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="9" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="13" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="17" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="21" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="36" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="38" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="31" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="32" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="33" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="35" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="36" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="37" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="38" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="44"/>
-    <cellStyle name="Nota" xfId="39" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="39" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Percent 2" xfId="57"/>
-    <cellStyle name="Saída" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Sheet Title" xfId="41"/>
-    <cellStyle name="Texto de Aviso" xfId="43" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="32" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="33" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="34" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="35" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="100">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="80">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2111,29 +1983,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="55.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="29.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="55.1640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1" s="4"/>
       <c r="D1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
@@ -2153,7 +2025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B3" s="18">
         <v>1</v>
       </c>
@@ -2174,7 +2046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B4" s="19">
         <f>B3+1</f>
         <v>2</v>
@@ -2196,7 +2068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:7" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B5" s="19">
         <f t="shared" ref="B5:B17" si="1">B4+1</f>
         <v>3</v>
@@ -2218,7 +2090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:7" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B6" s="19">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2240,7 +2112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B7" s="19">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2262,7 +2134,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B8" s="19">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2284,7 +2156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B9" s="19">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2306,7 +2178,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="19">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -2328,7 +2200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B11" s="19">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2350,7 +2222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="B12" s="19">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2372,7 +2244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B13" s="19">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2386,7 +2258,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="19">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2400,7 +2272,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="19">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2414,7 +2286,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="19">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2428,7 +2300,7 @@
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
     </row>
-    <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B17" s="19">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2442,273 +2314,273 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C18" s="9"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="99" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="74" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="75" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="76" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="77" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="78" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="94" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="69" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="71" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="71" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="72" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="72" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="73" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="89" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="64" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="65" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="66" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="66" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="67" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="67" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="68" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="84" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="59" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="60" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="61" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="61" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="62" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="62" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="63" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="63" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="79" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="54" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="55" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="56" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="57" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="58" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="74" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="49" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="50" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="51" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="52" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="52" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="53" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="69" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="44" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="46" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="47" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="48" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="64" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="39" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="40" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="41" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="42" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="43" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="43" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="59" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="34" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="36" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="37" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="38" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="38" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="54" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="31" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="32" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="33" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="49" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="26" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="27" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="28" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="44" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="21" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="22" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="23" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="39" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2729,26 +2601,26 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="6" width="8.85546875" style="1"/>
-    <col min="7" max="7" width="28.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="28.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="G2" s="16" t="s">
         <v>0</v>
       </c>
@@ -2759,7 +2631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="3">
         <f>B4+1</f>
         <v>3</v>
@@ -2782,7 +2654,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <f>B5+1</f>
         <v>2</v>
@@ -2799,7 +2671,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="14" t="s">
@@ -2809,7 +2681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -2825,7 +2697,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="14" t="s">
@@ -2835,7 +2707,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2850,7 +2722,7 @@
         <f>D6+1</f>
         <v>3</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="14" t="s">
@@ -2860,42 +2732,42 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G7" s="26" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G7" s="25" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G8" s="27" t="s">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G8" s="26" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:E5">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" stopIfTrue="1" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2906,4 +2778,762 @@
     <oddFooter>&amp;L&amp;FPMO Escritório de Projetos&amp;RPágina &amp;P de &amp;Nhttp://escritoriodeprojetos.com.br</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A1" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="29"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:P41"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[GPR] Atualizando a forma dos Recursos Humanos.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Quadro de Gerenciamento de Risco.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Quadro de Gerenciamento de Risco.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -159,8 +159,8 @@
 • Média – Valor 3 ou 4
 • Alta – Valor 5 ou 6
 Temos estratégias corretivas definidas para cada nível de prioridade de risco, sendo elas:
-Prioridade Baixa: Devem ser corrigidos dentro do prazo de 1 Sprint após ser diagnosticado e após a correção deve ser monitorado para evitar que volte a ocorrer.
-Prioridade Média: O responsável pela área de processo deve ter proposto uma opção de correção que deve ser analisada junto ao Gerente de Projeto e se aprovada, deve ser monitorada diariamente para que seja corrigida no prazo de uma semana e atualizado no Quadro de Gerenciamento de Riscos após ser devidamente corrigido.
+Prioridade Baixa:  Após ser diagnosticado e após a correção deve ser monitorado a cada sprint para evitar que volte a ocorrer.
+Prioridade Média: O responsável pela área de processo deve ter proposto uma opção de correção que deve ser analisada junto ao Gerente de Projeto e se aprovada, deve ser monitorada semanalmente e atualizado no Quadro de Gerenciamento de Riscos após ser devidamente corrigido.
 Prioridade Alta: O responsável pela área de processo deve ter proposto uma opção de correção que deve ser analisada junto ao Gerente de Projeto e se aprovada, deve ser monitorada diariamente para que seja corrigida o mais rápido possível e atualizado no Quadro de Gerenciamento de Riscos após ser devidamente corrigido.
 </t>
   </si>

</xml_diff>